<commit_message>
Updated quatt yaml files
</commit_message>
<xml_diff>
--- a/Quatt.xlsx
+++ b/Quatt.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\heatpumpcontroller\heatpump-listener-quatt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6331840-DC19-435B-AF3E-A57E9BB984C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E2F9023-EF21-48D1-B610-0622F6BF6A08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{ABECCABF-2B57-4433-85B2-4F1DE38595D0}"/>
   </bookViews>
@@ -516,10 +516,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9441A3DC-2F03-402E-AA72-39FB0A36C9FB}">
-  <dimension ref="A1:E41"/>
+  <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -527,7 +527,7 @@
     <col min="3" max="3" width="33.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -535,7 +535,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>42100</v>
       </c>
@@ -549,8 +549,15 @@
         <f t="shared" ref="E2:E12" si="0">A2-40001</f>
         <v>2099</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G2">
+        <v>1999</v>
+      </c>
+      <c r="H2">
+        <f>G2+40001</f>
+        <v>42000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>42101</v>
       </c>
@@ -564,8 +571,15 @@
         <f t="shared" si="0"/>
         <v>2100</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G3">
+        <v>3999</v>
+      </c>
+      <c r="H3">
+        <f>G3+40001</f>
+        <v>44000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>42102</v>
       </c>
@@ -579,8 +593,15 @@
         <f t="shared" si="0"/>
         <v>2101</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G4">
+        <v>2010</v>
+      </c>
+      <c r="H4">
+        <f>G4+40001</f>
+        <v>42011</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>42103</v>
       </c>
@@ -594,8 +615,15 @@
         <f t="shared" si="0"/>
         <v>2102</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G5">
+        <v>2015</v>
+      </c>
+      <c r="H5">
+        <f>G5+40001</f>
+        <v>42016</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>42104</v>
       </c>
@@ -610,7 +638,7 @@
         <v>2103</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>42105</v>
       </c>
@@ -625,7 +653,7 @@
         <v>2104</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>42106</v>
       </c>
@@ -640,7 +668,7 @@
         <v>2105</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>42107</v>
       </c>
@@ -652,7 +680,7 @@
         <v>2106</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>42108</v>
       </c>
@@ -667,7 +695,7 @@
         <v>2107</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>42109</v>
       </c>
@@ -682,7 +710,7 @@
         <v>2108</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>42110</v>
       </c>
@@ -695,7 +723,7 @@
         <v>2109</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>42111</v>
       </c>
@@ -710,7 +738,7 @@
         <v>2110</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>42112</v>
       </c>
@@ -725,7 +753,7 @@
         <v>2111</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>42113</v>
       </c>
@@ -740,7 +768,7 @@
         <v>2112</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>42114</v>
       </c>

</xml_diff>